<commit_message>
added logic for available & all, check donation
</commit_message>
<xml_diff>
--- a/uploadDonorDataToCloud/bloodDonorList.xlsx
+++ b/uploadDonorDataToCloud/bloodDonorList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropawar\Downloads\HO blood donor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyLearnings\HO-app\HO-BlooDonor\uploadDonorDataToCloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="68">
   <si>
     <t>city</t>
   </si>
@@ -144,6 +144,93 @@
   </si>
   <si>
     <t>MP</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Praveen</t>
+  </si>
+  <si>
+    <t>Pooja</t>
+  </si>
+  <si>
+    <t>Seeta</t>
+  </si>
+  <si>
+    <t>Geeta</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Deepak</t>
+  </si>
+  <si>
+    <t>Himanshu</t>
+  </si>
+  <si>
+    <t>Pathak</t>
+  </si>
+  <si>
+    <t>Dhyan</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>Moo</t>
+  </si>
+  <si>
+    <t>Sivahare</t>
+  </si>
+  <si>
+    <t>Rathi</t>
+  </si>
+  <si>
+    <t>Sharna</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>Kuvar</t>
+  </si>
+  <si>
+    <t>Pandit</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>katni</t>
+  </si>
+  <si>
+    <t>sihora</t>
+  </si>
+  <si>
+    <t>chhindwara</t>
+  </si>
+  <si>
+    <t>vijay nagar</t>
+  </si>
+  <si>
+    <t>Saori</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>15/12/2021</t>
+  </si>
+  <si>
+    <t>19/12/2021</t>
+  </si>
+  <si>
+    <t>15/1/2022</t>
   </si>
 </sst>
 </file>
@@ -179,8 +266,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,8 +620,8 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
-        <v>34</v>
+      <c r="G2" s="1">
+        <v>44807</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
@@ -567,8 +655,8 @@
       <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
-        <v>34</v>
+      <c r="G3" s="1">
+        <v>44564</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
@@ -577,7 +665,7 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="L3">
         <v>482005</v>
@@ -602,8 +690,8 @@
       <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
-        <v>33</v>
+      <c r="G4" s="1">
+        <v>44806</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -632,24 +720,374 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>1212121212</v>
+        <v>8923849283</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
-        <v>33</v>
+      <c r="G5" s="1">
+        <v>44805</v>
       </c>
       <c r="I5" t="s">
         <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
         <v>38</v>
       </c>
       <c r="L5">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2342342342</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44562</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2342342344</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44897</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>2312121111</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44806</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>9893894349</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>8898234234</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44805</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>4545454555</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44449</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>6767667677</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44450</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>7676767676</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44538</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>6766666666</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14">
+        <v>410101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>3434534553</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15">
         <v>410101</v>
       </c>
     </row>

</xml_diff>